<commit_message>
Final retriver top k accuracy results(single pdf/question)  for aws/hugging face embeddings models
</commit_message>
<xml_diff>
--- a/src/my_rag/evaluations/results/retriever_evaluation_results.xlsx
+++ b/src/my_rag/evaluations/results/retriever_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,26 +493,26 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'name': 'sentence-transformers/all-MiniLM-L6-v2', 'batch_size': 100}</t>
+          <t>{'name': 'sentence-transformers/all-MiniLM-L6-v2', 'batch_size': 100, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:'}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6307692307692307</v>
+        <v>0.5230769230769231</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7076923076923077</v>
+        <v>0.5692307692307692</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7230769230769231</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7384615384615385</v>
+        <v>0.676923076923077</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7846153846153846</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6874358974358974</v>
+        <v>0.5800000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -528,26 +528,26 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'name': 'mixedbread-ai/mxbai-embed-large-v1', 'batch_size': 100}</t>
+          <t>{'name': 'mixedbread-ai/mxbai-embed-large-v1', 'batch_size': 100, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:'}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.8615384615384616</v>
+        <v>0.4307692307692308</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9384615384615385</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9538461538461539</v>
+        <v>0.6461538461538462</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9538461538461539</v>
+        <v>0.676923076923077</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9538461538461539</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="I3" t="n">
-        <v>0.905128205128205</v>
+        <v>0.5312820512820513</v>
       </c>
     </row>
     <row r="4">
@@ -567,22 +567,22 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.9384615384615385</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9538461538461539</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9846153846153847</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9846153846153847</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9846153846153847</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9487179487179487</v>
+        <v>0.9641025641025641</v>
       </c>
     </row>
     <row r="5">
@@ -602,22 +602,22 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.2923076923076923</v>
+        <v>0.2769230769230769</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.6</v>
       </c>
       <c r="F5" t="n">
+        <v>0.6307692307692307</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.7076923076923077</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.7384615384615385</v>
-      </c>
       <c r="H5" t="n">
-        <v>0.7538461538461538</v>
+        <v>0.7076923076923077</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4953846153846154</v>
+        <v>0.467948717948718</v>
       </c>
     </row>
     <row r="6">
@@ -637,22 +637,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8153846153846154</v>
+        <v>0.8</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9076923076923077</v>
+        <v>0.8923076923076924</v>
       </c>
       <c r="F6" t="n">
+        <v>0.9384615384615385</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9384615384615385</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.9538461538461539</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.9538461538461539</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.9692307692307692</v>
-      </c>
       <c r="I6" t="n">
-        <v>0.88</v>
+        <v>0.8646153846153847</v>
       </c>
     </row>
     <row r="7">
@@ -663,7 +663,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PubMed filtered Dataset</t>
+          <t>HuggingFace QA Dataset</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -675,19 +675,19 @@
         <v>0.6923076923076923</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7692307692307693</v>
+        <v>0.7384615384615385</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.7384615384615385</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.7538461538461538</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.7846153846153846</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7564102564102563</v>
+        <v>0.7253846153846154</v>
       </c>
     </row>
     <row r="8">
@@ -698,7 +698,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PubMed filtered Dataset</t>
+          <t>HuggingFace QA Dataset</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.8769230769230769</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0.9282051282051281</v>
       </c>
     </row>
     <row r="9">
@@ -733,31 +733,31 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PubMed filtered Dataset</t>
+          <t>HuggingFace QA Dataset</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'name': 'nvidia/NV-Embed-v2', 'batch_size': 5, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:', 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True, 'max_length': 32768}}</t>
+          <t>{'name': 'nvidia/NV-Embed-v2', 'batch_size': 5, 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True, 'max_length': 32768}}</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.8769230769230769</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0.9384615384615385</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0.9538461538461539</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.9538461538461539</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0.9538461538461539</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0.9128205128205129</v>
       </c>
     </row>
     <row r="10">
@@ -768,31 +768,31 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PubMed filtered Dataset</t>
+          <t>HuggingFace QA Dataset</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'name': 'dunzhang/stella_en_1.5B_v5', 'batch_size': 20, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:', 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True}}</t>
+          <t>{'name': 'dunzhang/stella_en_1.5B_v5', 'batch_size': 20, 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True}}</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0.4153846153846154</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0.5230769230769231</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0.5846153846153846</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0.3651282051282051</v>
       </c>
     </row>
     <row r="11">
@@ -803,31 +803,381 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PubMed filtered Dataset</t>
+          <t>HuggingFace QA Dataset</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'name': 'amazon.titan-embed-text-v2:0', 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:', 'model_kwargs': {'aws': True, 'aws_creds_file': '/home/ubuntu/Multi-Agent-LLM-System-with-LangGraph-RAG-and-LangChain/config/config.ini', 'aws_config_name': 'BedRock_LLM_API'}}</t>
+          <t>{'name': 'amazon.titan-embed-text-v2:0', 'model_kwargs': {'aws': True, 'aws_creds_file': '/home/ubuntu/Multi-Agent-LLM-System-with-LangGraph-RAG-and-LangChain/config/config.ini', 'aws_config_name': 'BedRock_LLM_API'}}</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.9076923076923077</v>
       </c>
       <c r="F11" t="n">
         <v>0.9230769230769231</v>
       </c>
       <c r="G11" t="n">
+        <v>0.9538461538461539</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9538461538461539</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.8897435897435897</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>sentence-transformers/all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'name': 'sentence-transformers/all-MiniLM-L6-v2', 'batch_size': 100, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:'}</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.6538461538461539</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>mixedbread-ai/mxbai-embed-large-v1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'name': 'mixedbread-ai/mxbai-embed-large-v1', 'batch_size': 100, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:'}</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="F13" t="n">
         <v>0.9230769230769231</v>
       </c>
-      <c r="H11" t="n">
+      <c r="G13" t="n">
         <v>0.9230769230769231</v>
       </c>
-      <c r="I11" t="n">
+      <c r="H13" t="n">
         <v>0.9230769230769231</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.7948717948717949</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>nvidia/NV-Embed-v2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'name': 'nvidia/NV-Embed-v2', 'batch_size': 5, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:', 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True, 'max_length': 32768}}</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>dunzhang/stella_en_1.5B_v5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'name': 'dunzhang/stella_en_1.5B_v5', 'batch_size': 20, 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:', 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True}}</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>amazon.titan-embed-text-v2:0</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'name': 'amazon.titan-embed-text-v2:0', 'instruction': 'Instruct: Represent this passage for retrieval in response to relevant questions.\nQuery:', 'query_instruction': 'Instruct: Given a query, find the most relevant passages that can provide the answer.\nPassage:', 'model_kwargs': {'aws': True, 'aws_creds_file': '/home/ubuntu/Multi-Agent-LLM-System-with-LangGraph-RAG-and-LangChain/config/config.ini', 'aws_config_name': 'BedRock_LLM_API'}}</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>sentence-transformers/all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'name': 'sentence-transformers/all-MiniLM-L6-v2', 'batch_size': 100}</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.7564102564102563</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mixedbread-ai/mxbai-embed-large-v1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'name': 'mixedbread-ai/mxbai-embed-large-v1', 'batch_size': 100}</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>nvidia/NV-Embed-v2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'name': 'nvidia/NV-Embed-v2', 'batch_size': 5, 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True, 'max_length': 32768}}</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>dunzhang/stella_en_1.5B_v5</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'name': 'dunzhang/stella_en_1.5B_v5', 'batch_size': 20, 'model_kwargs': {'trust_remote_code': True, 'load_in_8bit': True}}</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>amazon.titan-embed-text-v2:0</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PubMed filtered Dataset</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'name': 'amazon.titan-embed-text-v2:0', 'model_kwargs': {'aws': True, 'aws_creds_file': '/home/ubuntu/Multi-Agent-LLM-System-with-LangGraph-RAG-and-LangChain/config/config.ini', 'aws_config_name': 'BedRock_LLM_API'}}</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>